<commit_message>
Update CCD configuration for Judgement store
</commit_message>
<xml_diff>
--- a/ccd_configuration/CCJ.xlsx
+++ b/ccd_configuration/CCJ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="196">
   <si>
     <t xml:space="preserve">Jurisdiction</t>
   </si>
@@ -75,13 +75,13 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">CIVILENFORCEMENT</t>
+    <t xml:space="preserve">CET</t>
   </si>
   <si>
     <t xml:space="preserve">Civil Enforcement</t>
   </si>
   <si>
-    <t xml:space="preserve">Validate and issue county court judgements</t>
+    <t xml:space="preserve">Show County Court Judgements</t>
   </si>
   <si>
     <t xml:space="preserve">CaseType</t>
@@ -145,22 +145,13 @@
     <t xml:space="preserve">DisplayOrder</t>
   </si>
   <si>
-    <t xml:space="preserve">CCJDetailsAdded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCJ details added</t>
-  </si>
-  <si>
-    <t xml:space="preserve">County Court Judgement details added</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCJDetailsValidated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCJ details validated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">County Court Judgement details validated</t>
+    <t xml:space="preserve">CCJDetailsRetrieved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCJ details retrieved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">County Court Judgement details retrieved from CaseMan</t>
   </si>
   <si>
     <t xml:space="preserve">CaseEvent</t>
@@ -239,7 +230,10 @@
     <t xml:space="preserve">EndButtonLabel</t>
   </si>
   <si>
-    <t xml:space="preserve">addJudgementDetails</t>
+    <t xml:space="preserve">retrieveJudgementDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrieve judgement details</t>
   </si>
   <si>
     <t xml:space="preserve">Public</t>
@@ -251,12 +245,6 @@
     <t xml:space="preserve">Save and Continue</t>
   </si>
   <si>
-    <t xml:space="preserve">validateJudgement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submit</t>
-  </si>
-  <si>
     <t xml:space="preserve">CaseField</t>
   </si>
   <si>
@@ -314,12 +302,18 @@
     <t xml:space="preserve">Judgement date</t>
   </si>
   <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">judgementAmount</t>
   </si>
   <si>
     <t xml:space="preserve">Judgement amount</t>
   </si>
   <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">interestCosts</t>
   </si>
   <si>
@@ -347,7 +341,7 @@
     <t xml:space="preserve">defendantName</t>
   </si>
   <si>
-    <t xml:space="preserve">Defendant name</t>
+    <t xml:space="preserve">Defendant fullname</t>
   </si>
   <si>
     <t xml:space="preserve">defendantAddress</t>
@@ -356,10 +350,13 @@
     <t xml:space="preserve">Defendant address</t>
   </si>
   <si>
+    <t xml:space="preserve">AddressUK</t>
+  </si>
+  <si>
     <t xml:space="preserve">claimantName</t>
   </si>
   <si>
-    <t xml:space="preserve">Claimant</t>
+    <t xml:space="preserve">Claimant fullname</t>
   </si>
   <si>
     <t xml:space="preserve">claimantAddress</t>
@@ -368,12 +365,6 @@
     <t xml:space="preserve">Claimant address</t>
   </si>
   <si>
-    <t xml:space="preserve">claimDecision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Claim decision</t>
-  </si>
-  <si>
     <t xml:space="preserve">ComplexTypes</t>
   </si>
   <si>
@@ -416,28 +407,22 @@
     <t xml:space="preserve">Part admission</t>
   </si>
   <si>
+    <t xml:space="preserve">deteminationByJudgeJudgementType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determination by judge</t>
+  </si>
+  <si>
     <t xml:space="preserve">paidJudgementStatus</t>
   </si>
   <si>
-    <t xml:space="preserve">Paid</t>
+    <t xml:space="preserve">Satisfied</t>
   </si>
   <si>
     <t xml:space="preserve">unpaidJudgementStatus</t>
   </si>
   <si>
-    <t xml:space="preserve">Unpaid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acceptedClaimDecision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accepted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rejectedClaimDecision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rejected</t>
+    <t xml:space="preserve">Cancelled</t>
   </si>
   <si>
     <t xml:space="preserve">CaseEventToFields</t>
@@ -518,10 +503,7 @@
     <t xml:space="preserve">Judgement details</t>
   </si>
   <si>
-    <t xml:space="preserve">judgementValidation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Judgement validation</t>
+    <t xml:space="preserve">OPTIONAL</t>
   </si>
   <si>
     <t xml:space="preserve">SearchInputFields</t>
@@ -533,6 +515,9 @@
     <t xml:space="preserve">Claimant name</t>
   </si>
   <si>
+    <t xml:space="preserve">Defendant name</t>
+  </si>
+  <si>
     <t xml:space="preserve">SearchResultFields</t>
   </si>
   <si>
@@ -611,6 +596,9 @@
     <t xml:space="preserve">test.caseworker@hmcts.net</t>
   </si>
   <si>
+    <t xml:space="preserve">caseworker.cet@hmcts.net</t>
+  </si>
+  <si>
     <t xml:space="preserve">AuthorisationCaseType</t>
   </si>
   <si>
@@ -626,16 +614,16 @@
     <t xml:space="preserve">CRUD</t>
   </si>
   <si>
-    <t xml:space="preserve">caseworker-test-junior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caseworker-test-solicitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caseworker-test-senior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caseworker-test-manager</t>
+    <t xml:space="preserve">caseworker-cet-junior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caseworker-cet-solicitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caseworker-cet-senior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caseworker-cet-manager</t>
   </si>
   <si>
     <t xml:space="preserve">AuthorisationCaseField</t>
@@ -1471,7 +1459,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1493,16 +1481,16 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G2" s="35"/>
       <c r="H2" s="35"/>
@@ -1537,10 +1525,10 @@
         <v>32</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>33</v>
@@ -1576,10 +1564,10 @@
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F4" s="5" t="n">
         <v>1</v>
@@ -1615,10 +1603,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F5" s="5" t="n">
         <v>2</v>
@@ -1654,10 +1642,10 @@
         <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F6" s="5" t="n">
         <v>3</v>
@@ -1693,10 +1681,10 @@
         <v>25</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="F7" s="5" t="n">
         <v>4</v>
@@ -1751,7 +1739,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1766,7 +1754,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>1</v>
@@ -1784,16 +1772,16 @@
       <c r="A2" s="46"/>
       <c r="B2" s="46"/>
       <c r="C2" s="47" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1807,10 +1795,10 @@
         <v>32</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F3" s="48" t="s">
         <v>33</v>
@@ -1824,13 +1812,13 @@
       <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="21" t="n">
+      <c r="D4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1886,7 +1874,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1906,16 +1894,16 @@
     </row>
     <row r="2" s="13" customFormat="true" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,10 +1917,10 @@
         <v>32</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>33</v>
@@ -1968,10 +1956,10 @@
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F4" s="21" t="n">
         <v>1</v>
@@ -2007,10 +1995,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F5" s="5" t="n">
         <v>2</v>
@@ -2046,10 +2034,10 @@
         <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F6" s="5" t="n">
         <v>3</v>
@@ -2085,10 +2073,10 @@
         <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="F7" s="21" t="n">
         <v>4</v>
@@ -2142,8 +2130,8 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K29" activeCellId="0" sqref="K29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2165,7 +2153,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="9" t="s">
@@ -2194,16 +2182,16 @@
         <v>4</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2217,31 +2205,31 @@
         <v>32</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="K3" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -2269,19 +2257,19 @@
         <v>25</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I4" s="49"/>
       <c r="J4" s="24" t="n">
@@ -2300,19 +2288,19 @@
         <v>25</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J5" s="24" t="n">
         <v>2</v>
@@ -2329,19 +2317,19 @@
         <v>25</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I6" s="21"/>
       <c r="J6" s="24" t="n">
@@ -2359,19 +2347,19 @@
         <v>25</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="24" t="n">
@@ -2390,19 +2378,19 @@
         <v>25</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J8" s="24" t="n">
         <v>5</v>
@@ -2420,19 +2408,19 @@
         <v>25</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G9" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I9" s="49"/>
       <c r="J9" s="24" t="n">
@@ -2451,19 +2439,19 @@
         <v>25</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I10" s="49"/>
       <c r="J10" s="24" t="n">
@@ -2482,19 +2470,19 @@
         <v>25</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G11" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I11" s="49"/>
       <c r="J11" s="24" t="n">
@@ -2513,19 +2501,19 @@
         <v>25</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I12" s="49"/>
       <c r="J12" s="24" t="n">
@@ -2544,19 +2532,19 @@
         <v>25</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G13" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I13" s="49"/>
       <c r="J13" s="24" t="n">
@@ -2575,19 +2563,19 @@
         <v>25</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I14" s="49"/>
       <c r="J14" s="24" t="n">
@@ -2606,19 +2594,19 @@
         <v>25</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G15" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I15" s="49"/>
       <c r="J15" s="24" t="n">
@@ -2628,33 +2616,7 @@
       <c r="L15" s="24"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2710,11 +2672,11 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A16" type="date">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A15" type="date">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" prompt="Enter a date after 'LiveFrom' date" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4:B16" type="none">
+    <dataValidation allowBlank="true" operator="equal" prompt="Enter a date after 'LiveFrom' date" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4:B15" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2736,8 +2698,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2753,7 +2715,7 @@
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2780,24 +2742,24 @@
         <v>8</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="n">
-        <v>43101</v>
+        <v>43405</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>12</v>
@@ -2811,10 +2773,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="n">
-        <v>43101</v>
+        <v>43405</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>12</v>
@@ -2826,6 +2788,25 @@
         <v>34</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="n">
+        <v>43405</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2877,14 +2858,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2907,10 +2888,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,10 +2905,10 @@
         <v>32</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2939,10 +2920,10 @@
         <v>25</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F4" s="5"/>
     </row>
@@ -2955,10 +2936,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F5" s="5"/>
     </row>
@@ -2971,10 +2952,10 @@
         <v>25</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2986,10 +2967,10 @@
         <v>25</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3014,10 +2995,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA55"/>
+  <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3026,14 +3007,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -3063,7 +3044,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -3098,13 +3079,13 @@
         <v>32</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3116,13 +3097,13 @@
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,13 +3114,13 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3150,13 +3131,13 @@
         <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3167,13 +3148,13 @@
         <v>25</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3184,13 +3165,13 @@
         <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3201,13 +3182,13 @@
         <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3218,13 +3199,13 @@
         <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3235,13 +3216,13 @@
         <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,13 +3233,13 @@
         <v>25</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3269,13 +3250,13 @@
         <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3286,13 +3267,13 @@
         <v>25</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3303,31 +3284,20 @@
         <v>25</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>190</v>
-      </c>
+      <c r="A16" s="10"/>
+      <c r="C16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="n">
@@ -3338,13 +3308,13 @@
         <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3355,13 +3325,13 @@
         <v>25</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,13 +3342,13 @@
         <v>25</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3389,13 +3359,13 @@
         <v>25</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3406,13 +3376,13 @@
         <v>25</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3423,13 +3393,13 @@
         <v>25</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3440,13 +3410,13 @@
         <v>25</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3457,13 +3427,13 @@
         <v>25</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3474,13 +3444,13 @@
         <v>25</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3491,13 +3461,13 @@
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3508,13 +3478,13 @@
         <v>25</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3525,31 +3495,19 @@
         <v>25</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>190</v>
-      </c>
+      <c r="A29" s="10"/>
+      <c r="C29" s="5"/>
+      <c r="F29" s="24"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="n">
@@ -3560,13 +3518,13 @@
         <v>25</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3577,13 +3535,13 @@
         <v>25</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3594,13 +3552,13 @@
         <v>25</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3611,13 +3569,13 @@
         <v>25</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3628,13 +3586,13 @@
         <v>25</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3645,13 +3603,13 @@
         <v>25</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3662,13 +3620,13 @@
         <v>25</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3679,13 +3637,13 @@
         <v>25</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3696,13 +3654,13 @@
         <v>25</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3713,13 +3671,13 @@
         <v>25</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3730,13 +3688,13 @@
         <v>25</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3747,31 +3705,19 @@
         <v>25</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>190</v>
-      </c>
+      <c r="A42" s="10"/>
+      <c r="C42" s="5"/>
+      <c r="F42" s="24"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="n">
@@ -3782,13 +3728,13 @@
         <v>25</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3799,13 +3745,13 @@
         <v>25</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3816,13 +3762,13 @@
         <v>25</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3833,13 +3779,13 @@
         <v>25</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3850,13 +3796,13 @@
         <v>25</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3867,13 +3813,13 @@
         <v>25</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3884,13 +3830,13 @@
         <v>25</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3901,13 +3847,13 @@
         <v>25</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3918,13 +3864,13 @@
         <v>25</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3935,13 +3881,13 @@
         <v>25</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3952,13 +3898,13 @@
         <v>25</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3969,35 +3915,18 @@
         <v>25</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="F55" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A55" type="date">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A54" type="date">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4020,7 +3949,7 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4029,13 +3958,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4063,10 +3992,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -4101,13 +4030,13 @@
         <v>32</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4118,13 +4047,13 @@
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4135,13 +4064,13 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4152,13 +4081,13 @@
         <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4169,87 +4098,19 @@
         <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4272,7 +4133,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A11" type="date">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A7" type="date">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4295,7 +4156,7 @@
   <dimension ref="A1:IU1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K29" activeCellId="0" sqref="K29"/>
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4304,14 +4165,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="51" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="51" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="51" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="51" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="51" width="31.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="6" style="51" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="256" style="51" width="8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="52" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B1" s="53" t="s">
         <v>1</v>
@@ -4583,10 +4444,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="60" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F2" s="60" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G2" s="59"/>
       <c r="H2" s="59"/>
@@ -4849,13 +4710,13 @@
         <v>32</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E3" s="64" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G3" s="56"/>
       <c r="H3" s="56"/>
@@ -5119,10 +4980,10 @@
         <v>34</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5137,10 +4998,10 @@
         <v>34</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5155,10 +5016,10 @@
         <v>34</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5173,84 +5034,16 @@
         <v>34</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5272,7 +5065,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A11" type="date">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A7" type="date">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5295,7 +5088,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5582,26 +5375,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5609,7 +5385,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A5" type="date">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4" type="date">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5639,8 +5415,8 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5670,7 +5446,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -5691,40 +5467,40 @@
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="J2" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>46</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="O2" s="15" t="s">
         <v>19</v>
@@ -5733,16 +5509,16 @@
         <v>20</v>
       </c>
       <c r="Q2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="22" t="s">
         <v>47</v>
-      </c>
-      <c r="R2" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" s="22" t="s">
-        <v>50</v>
       </c>
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
@@ -5777,43 +5553,43 @@
         <v>33</v>
       </c>
       <c r="H3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>55</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>58</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="Q3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="R3" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="S3" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="23" t="s">
         <v>59</v>
-      </c>
-      <c r="R3" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="S3" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="T3" s="23" t="s">
-        <v>62</v>
       </c>
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
@@ -5834,13 +5610,13 @@
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>1</v>
@@ -5855,57 +5631,19 @@
       <c r="M4" s="5"/>
       <c r="N4" s="25"/>
       <c r="P4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="T4" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="Q4" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="R5" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="T5" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5916,7 +5654,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A5" type="date">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4" type="date">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5924,7 +5662,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" prompt="Enter a value that is after LiveFrom date" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4:B5" type="none">
+    <dataValidation allowBlank="true" operator="equal" prompt="Enter a value that is after LiveFrom date" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5946,8 +5684,8 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5968,7 +5706,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -5989,25 +5727,25 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>20</v>
@@ -6043,28 +5781,28 @@
         <v>9</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -6090,14 +5828,14 @@
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H4" s="5"/>
       <c r="J4" s="5" t="s">
@@ -6116,17 +5854,17 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>28</v>
@@ -6141,14 +5879,14 @@
         <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H6" s="21"/>
       <c r="J6" s="5" t="s">
@@ -6164,14 +5902,14 @@
         <v>25</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="21" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H7" s="5"/>
       <c r="J7" s="5" t="s">
@@ -6187,14 +5925,14 @@
         <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="21" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H8" s="5"/>
       <c r="J8" s="5" t="s">
@@ -6210,13 +5948,13 @@
         <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -6233,17 +5971,17 @@
         <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>28</v>
@@ -6258,14 +5996,14 @@
         <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="21" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H11" s="21"/>
       <c r="J11" s="5" t="s">
@@ -6281,14 +6019,14 @@
         <v>25</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H12" s="5"/>
       <c r="J12" s="5" t="s">
@@ -6304,14 +6042,14 @@
         <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="21" t="s">
-        <v>82</v>
       </c>
       <c r="H13" s="5"/>
       <c r="J13" s="5" t="s">
@@ -6326,13 +6064,13 @@
         <v>25</v>
       </c>
       <c r="D14" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>103</v>
-      </c>
       <c r="G14" s="21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H14" s="21"/>
       <c r="J14" s="5" t="s">
@@ -6347,41 +6085,19 @@
         <v>25</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>82</v>
+      <c r="G15" s="0" t="s">
+        <v>100</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6419,7 +6135,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A16" type="date">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A15" type="date">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6468,7 +6184,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -6491,31 +6207,31 @@
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>31</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L2" s="14" t="s">
         <v>20</v>
@@ -6548,37 +6264,37 @@
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
@@ -6618,14 +6334,15 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="30.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="0" width="8.71"/>
@@ -6633,7 +6350,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -6655,13 +6372,13 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -6697,10 +6414,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -6730,13 +6447,13 @@
         <v>43405</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6744,27 +6461,27 @@
         <v>43405</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>94</v>
+      <c r="C6" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6772,13 +6489,13 @@
         <v>43405</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6786,30 +6503,17 @@
         <v>43405</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6826,7 +6530,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A9" type="date">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A8" type="date">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6848,8 +6552,8 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P18" activeCellId="0" sqref="P18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6875,7 +6579,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -6897,43 +6601,43 @@
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="J2" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="K2" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="N2" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="O2" s="22" t="s">
         <v>135</v>
-      </c>
-      <c r="I2" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>140</v>
       </c>
       <c r="P2" s="29"/>
       <c r="Q2" s="29"/>
@@ -6960,40 +6664,40 @@
         <v>32</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="J3" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="K3" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="L3" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="N3" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="O3" s="34" t="s">
         <v>146</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="L3" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="M3" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="N3" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="O3" s="34" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7005,23 +6709,23 @@
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F4" s="24" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K4" s="5" t="n">
         <v>1</v>
@@ -7040,23 +6744,23 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F5" s="24" t="n">
         <v>2</v>
       </c>
       <c r="G5" s="24"/>
       <c r="H5" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K5" s="5" t="n">
         <v>1</v>
@@ -7071,22 +6775,22 @@
         <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F6" s="24" t="n">
         <v>3</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K6" s="5" t="n">
         <v>1</v>
@@ -7105,22 +6809,22 @@
         <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F7" s="24" t="n">
         <v>4</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K7" s="5" t="n">
         <v>1</v>
@@ -7139,23 +6843,23 @@
         <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" s="24" t="n">
         <v>5</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K8" s="5" t="n">
         <v>1</v>
@@ -7170,23 +6874,23 @@
         <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F9" s="24" t="n">
         <v>6</v>
       </c>
       <c r="G9" s="24"/>
       <c r="H9" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K9" s="5" t="n">
         <v>1</v>
@@ -7201,22 +6905,22 @@
         <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F10" s="24" t="n">
         <v>7</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K10" s="5" t="n">
         <v>1</v>
@@ -7235,22 +6939,22 @@
         <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F11" s="24" t="n">
         <v>8</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K11" s="5" t="n">
         <v>1</v>
@@ -7269,23 +6973,23 @@
         <v>25</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F12" s="24" t="n">
         <v>9</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K12" s="5" t="n">
         <v>1</v>
@@ -7300,23 +7004,23 @@
         <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F13" s="24" t="n">
         <v>10</v>
       </c>
       <c r="G13" s="24"/>
       <c r="H13" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K13" s="5" t="n">
         <v>1</v>
@@ -7331,22 +7035,22 @@
         <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F14" s="24" t="n">
         <v>11</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K14" s="5" t="n">
         <v>1</v>
@@ -7365,22 +7069,22 @@
         <v>25</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F15" s="24" t="n">
         <v>12</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K15" s="5" t="n">
         <v>1</v>
@@ -7390,37 +7094,8 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
-        <v>43405</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7429,7 +7104,7 @@
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7437,7 +7112,7 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7449,7 +7124,7 @@
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7463,7 +7138,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A16" type="date">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" prompt="Enter a date on or after 01/01/2017" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A15" type="date">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7504,7 +7179,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -7526,16 +7201,16 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G2" s="35"/>
       <c r="H2" s="35"/>
@@ -7570,10 +7245,10 @@
         <v>32</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>33</v>
@@ -7609,10 +7284,10 @@
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F4" s="5" t="n">
         <v>1</v>
@@ -7648,10 +7323,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F5" s="5" t="n">
         <v>2</v>
@@ -7686,10 +7361,10 @@
         <v>25</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>3</v>

</xml_diff>